<commit_message>
ändringar och kompletteringar av .xlsx fil med förslag till menyer mm
</commit_message>
<xml_diff>
--- a/dokument/SkidTavling.xlsx
+++ b/dokument/SkidTavling.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="25440" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="25440" windowHeight="12600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="4" r:id="rId1"/>
     <sheet name="Tavling" sheetId="1" r:id="rId2"/>
     <sheet name="Deltagare" sheetId="2" r:id="rId3"/>
-    <sheet name="Blad3" sheetId="3" r:id="rId4"/>
+    <sheet name="handelselogg" sheetId="3" r:id="rId4"/>
+    <sheet name="Menyförteckning" sheetId="5" r:id="rId5"/>
+    <sheet name="dIV FÖRSLAG" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="160">
   <si>
     <t>åtkomst</t>
   </si>
@@ -88,9 +90,6 @@
     <t>long</t>
   </si>
   <si>
-    <t>startIntervall</t>
-  </si>
-  <si>
     <t>Beskrivning/klass public</t>
   </si>
   <si>
@@ -212,13 +211,301 @@
   </si>
   <si>
     <t>kontroll av postens integritet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abstract klass Enum </t>
+  </si>
+  <si>
+    <t>class participantStatus</t>
+  </si>
+  <si>
+    <t>ANMALD</t>
+  </si>
+  <si>
+    <t>BETALTAVG</t>
+  </si>
+  <si>
+    <t>NARVARANDESTARTPLATS</t>
+  </si>
+  <si>
+    <t>STARTAD</t>
+  </si>
+  <si>
+    <t>MELLANTID</t>
+  </si>
+  <si>
+    <t>MALGANG</t>
+  </si>
+  <si>
+    <t>AVBRUTIT</t>
+  </si>
+  <si>
+    <t>AVANMALD</t>
+  </si>
+  <si>
+    <t>HASHCODE</t>
+  </si>
+  <si>
+    <t>Ersätter ett antal boolean</t>
+  </si>
+  <si>
+    <t>class tavlingStartmetod</t>
+  </si>
+  <si>
+    <t>MASSTART</t>
+  </si>
+  <si>
+    <t>JAKTSTART</t>
+  </si>
+  <si>
+    <t>INDIVSTART</t>
+  </si>
+  <si>
+    <t>RANDOMSTART</t>
+  </si>
+  <si>
+    <t>ERSÄTTES TEX AV ENUM</t>
+  </si>
+  <si>
+    <t>int  startMetod</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>startMetod</t>
+  </si>
+  <si>
+    <t>hashcode</t>
+  </si>
+  <si>
+    <t>fel skall vara deltagare</t>
+  </si>
+  <si>
+    <t>startIntervall, sekunder</t>
+  </si>
+  <si>
+    <t>HANDELSELOGG</t>
+  </si>
+  <si>
+    <t>seqNr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">löpande nummer </t>
+  </si>
+  <si>
+    <t>regSrce</t>
+  </si>
+  <si>
+    <t>Rutin som rapporterat</t>
+  </si>
+  <si>
+    <t>Huvudmenyns nummer för källnummer</t>
+  </si>
+  <si>
+    <t>tidStampel</t>
+  </si>
+  <si>
+    <t>när..</t>
+  </si>
+  <si>
+    <t>Handkod</t>
+  </si>
+  <si>
+    <t>se tex nedan</t>
+  </si>
+  <si>
+    <t>illustration till fördelarna med enum</t>
+  </si>
+  <si>
+    <t>förklarar vad koden betyder, förhindrar misstag.</t>
+  </si>
+  <si>
+    <t>enum Handelsekod</t>
+  </si>
+  <si>
+    <t>NYDELT</t>
+  </si>
+  <si>
+    <t>REGANKOMST</t>
+  </si>
+  <si>
+    <t>REGSTART</t>
+  </si>
+  <si>
+    <t>REGMELLAN</t>
+  </si>
+  <si>
+    <t>REGMAL</t>
+  </si>
+  <si>
+    <t>FALLOLYCKA</t>
+  </si>
+  <si>
+    <t>VADEROMSLAG</t>
+  </si>
+  <si>
+    <t>AVBROTT</t>
+  </si>
+  <si>
+    <t>ANMALANSTANGD</t>
+  </si>
+  <si>
+    <t>VINNAREUTSEDD</t>
+  </si>
+  <si>
+    <t>DISKVAL</t>
+  </si>
+  <si>
+    <t>DOMMARUTSLAG</t>
+  </si>
+  <si>
+    <t>ANNANHAND</t>
+  </si>
+  <si>
+    <t>OVR1</t>
+  </si>
+  <si>
+    <t>OVR2</t>
+  </si>
+  <si>
+    <t>OVR3</t>
+  </si>
+  <si>
+    <t>berStartnr</t>
+  </si>
+  <si>
+    <t>ev relaterad åkare</t>
+  </si>
+  <si>
+    <t>annat ID</t>
+  </si>
+  <si>
+    <t>innan utdelning #</t>
+  </si>
+  <si>
+    <t>1. TÄVLING</t>
+  </si>
+  <si>
+    <t>MENY</t>
+  </si>
+  <si>
+    <t>UNDERMENY</t>
+  </si>
+  <si>
+    <t>FÖRKLARING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ändra registrera egenskaper som inte kan hårdkodas. Av olika skäl. Tex datum, startmetod o simuleringskod. </t>
+  </si>
+  <si>
+    <t>2.DELTAGARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ladda deltagarfil, </t>
+  </si>
+  <si>
+    <t>2.1 Ladda fil med namn</t>
+  </si>
+  <si>
+    <t>2.2 Ta emot nyanmälan</t>
+  </si>
+  <si>
+    <t>tänkbart alternativ ny deltagare som inte fanns i filen</t>
+  </si>
+  <si>
+    <t>3. LÅS DELTAGARLISTA</t>
+  </si>
+  <si>
+    <t>INGA FLER ÄNDRINGAR ELLER TILLÄGG</t>
+  </si>
+  <si>
+    <t>Programmet förberder för start genom att beräkna dela utt starttider och startnummer till deltagarna.</t>
+  </si>
+  <si>
+    <t>4. STARTLISTA</t>
+  </si>
+  <si>
+    <t>4.1 SKRIVA UT HELA</t>
+  </si>
+  <si>
+    <t>4.2  ENSKILDS STARTDAT</t>
+  </si>
+  <si>
+    <t>LISTA DELTAGARE MED STARTNUMMER OCH TID.</t>
+  </si>
+  <si>
+    <t>VISA ENSKILDS UTIFRÅN NAMN ELLER ANM NUMMER. (STARTNUMMER OKÄNT)</t>
+  </si>
+  <si>
+    <t>5. STARTA</t>
+  </si>
+  <si>
+    <t>AUTOMTATISK START. START BOKAS SOM KALKYLERD STARTTIDPUNKT.</t>
+  </si>
+  <si>
+    <t>5.1 ÖVERKURS</t>
+  </si>
+  <si>
+    <t>RAPPORTERA AVVIKELSER SOM TJYVSTART, UTEBLIVEN ELLER SEN START.</t>
+  </si>
+  <si>
+    <t>6.MELLANTIDER</t>
+  </si>
+  <si>
+    <t>OM SIM VALD; KAN ENSKILD DELTAGARES KALKYLERADE TID ÄNDRAS MANUELLT</t>
+  </si>
+  <si>
+    <t>7. MÅLGÅNG</t>
+  </si>
+  <si>
+    <t>SOM MELLANTIDER VID SIMULERAD KAN KALKYLERAD ÄNDRAS.</t>
+  </si>
+  <si>
+    <t>8. AVSLUT  PRISUTDELNING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VID SIMULERING AUTOMATISK, NÄR ALLAS MÅLLGÅNG KONSTATERATS. BERÄKNA ORDNING MED ÅKTID SOM GRUND. BERÄKNA TRE </t>
+  </si>
+  <si>
+    <t>FÖRSTA PLATSER. SKAPA UNDERLAG FÖR UTSKRIFT</t>
+  </si>
+  <si>
+    <t>9. UTSKRIFTER</t>
+  </si>
+  <si>
+    <t>9.1. DELTAGARE</t>
+  </si>
+  <si>
+    <t>9.2. DELTAGARE I STARTORDNING</t>
+  </si>
+  <si>
+    <t>9.3 DELTAGARE MELLANTIDER</t>
+  </si>
+  <si>
+    <t>9.4. DELTAGARE PLACERING I MÅL ÅKTID</t>
+  </si>
+  <si>
+    <t>10.X-TRA</t>
+  </si>
+  <si>
+    <t>10.1 DELTAGARGRUPP JÄMFÖRELSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* SE "GRUNDLÄGGANDE KRAV" PLACERING VID MELLANTIDER ? FRÅGAN KRÄVER NOG YTTERLIGARE UTREDNING VAD SOM AVSES. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VID SIMULERING KAN RESULTAT FINNAS REDAN FÖRE START?. AVSES KLUNGA </t>
+  </si>
+  <si>
+    <t>ALL UTSKRIFT PÅ KONSOLEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,8 +513,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,8 +563,33 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -249,11 +597,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -268,8 +651,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Anteckning" xfId="5" builtinId="10"/>
+    <cellStyle name="Beräkning" xfId="4" builtinId="22"/>
+    <cellStyle name="Bra" xfId="1" builtinId="26"/>
+    <cellStyle name="Dålig" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -538,13 +941,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>2305050</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -554,8 +957,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1104900" y="5800725"/>
-          <a:ext cx="10134600" cy="3981450"/>
+          <a:off x="1104900" y="8105775"/>
+          <a:ext cx="10134600" cy="1676400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -600,6 +1003,277 @@
         </a:p>
         <a:p>
           <a:endParaRPr lang="sv-SE" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="textruta 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123825" y="1219200"/>
+          <a:ext cx="5581650" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100"/>
+            <a:t>FÖR BLA FUNKTIONSKONTROLL,DEBUGGING MED MERA FÖRESLÅR JAG EN NY KLASS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100"/>
+            <a:t>"HÄNDELSER" I PRINCIP EN LOGGFIL, SOM  INNEHÅLLER </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
+            <a:t> EN RAD FÖR VARJE HÄNDELSE, SMÅ PROBLEM OM MAN KÖR I EN ENDA APPLIKATION. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
+            <a:t>även för handläggning av klagomål mot tävlinsledningen  mm.</a:t>
+          </a:r>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7696200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="textruta 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="4914900"/>
+          <a:ext cx="10467975" cy="1857375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100"/>
+            <a:t>FÖRSLAG TILL MENYER SKIDTÄVLING.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100"/>
+            <a:t>2021-12-04;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="textruta 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="285751"/>
+          <a:ext cx="6096000" cy="1466850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100"/>
+            <a:t>1. DET FINNS FLERA SÄTT ATT HANTERA FRÅGAN HUR MAN HITTAR RÄTT DELTAGARE FÖR REISTRERING </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100"/>
+            <a:t>AV OLIKA HÄNDELSER. eN ÄR ATT LÄSA IGENOM LISTAN EFTER DEN SÖKTA POSTEN, TEX VISST STARTNUMMER FÖR REG AV MELLANTID, MÅLTID.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100"/>
+            <a:t>EN</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
+            <a:t> ANNAN ÄR ARR GÖRA EN TABELL DÄR POSITION I TABELL- ARRAYEN  MOTSVARAR STARTNUMMER OCH ARRAYENS INNEHÅLL PÅ DEN POSITIONEN ÖR DELTAGAREN MED DET STARTNUMMRET. EN SORTS INDEX. MED FÅ DELTAGARE SPELAR VALET MINDRE ROLL; MEN NÅGON FORM AV METOD ÄR BRA ATT HA.</a:t>
+          </a:r>
+          <a:endParaRPr lang="sv-SE" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -895,7 +1569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
@@ -908,10 +1582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -929,13 +1603,13 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
@@ -975,58 +1649,67 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="12" customFormat="1" ht="18" customHeight="1">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="F4" s="13" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1">
-      <c r="A5" t="s">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="F5" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1">
-      <c r="A6" t="s">
+      <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="F6" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1">
-      <c r="A7" t="s">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1">
-      <c r="A8" t="s">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1087,7 +1770,7 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1"/>
@@ -1099,19 +1782,19 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" t="s">
         <v>32</v>
       </c>
-      <c r="G16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1119,47 +1802,99 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
         <v>61</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" t="s">
         <v>63</v>
       </c>
-      <c r="G17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1">
+      <c r="H17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18" customHeight="1">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
       </c>
       <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1"/>
-    <row r="20" spans="1:7" ht="18" customHeight="1"/>
-    <row r="21" spans="1:7" ht="18" customHeight="1"/>
-    <row r="22" spans="1:7" ht="18" customHeight="1"/>
-    <row r="23" spans="1:7" ht="18" customHeight="1"/>
-    <row r="24" spans="1:7" ht="18" customHeight="1"/>
-    <row r="25" spans="1:7" ht="18" customHeight="1"/>
-    <row r="26" spans="1:7" ht="18" customHeight="1"/>
-    <row r="27" spans="1:7" ht="18" customHeight="1"/>
-    <row r="28" spans="1:7" ht="18" customHeight="1"/>
-    <row r="29" spans="1:7" ht="18" customHeight="1"/>
-    <row r="30" spans="1:7" ht="18" customHeight="1"/>
-    <row r="31" spans="1:7" ht="18" customHeight="1"/>
-    <row r="32" spans="1:7" ht="18" customHeight="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" customHeight="1"/>
+    <row r="20" spans="1:8" ht="18" customHeight="1"/>
+    <row r="21" spans="1:8" ht="18" customHeight="1">
+      <c r="A21" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18" customHeight="1"/>
+    <row r="23" spans="1:8" ht="18" customHeight="1"/>
+    <row r="24" spans="1:8" ht="18" customHeight="1"/>
+    <row r="25" spans="1:8" ht="18" customHeight="1"/>
+    <row r="26" spans="1:8" ht="18" customHeight="1">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18" customHeight="1">
+      <c r="A27" s="6">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18" customHeight="1">
+      <c r="A28" s="6">
+        <v>2</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18" customHeight="1">
+      <c r="A29" s="6">
+        <v>3</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18" customHeight="1">
+      <c r="A30" s="7">
+        <v>4</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18" customHeight="1"/>
+    <row r="32" spans="1:8" ht="18" customHeight="1"/>
     <row r="33" ht="18" customHeight="1"/>
+    <row r="34" ht="18" customHeight="1"/>
+    <row r="35" ht="18" customHeight="1"/>
+    <row r="36" ht="18" customHeight="1"/>
+    <row r="37" ht="18" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1169,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A7" sqref="A7:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1220,121 +1955,126 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" t="s">
         <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1345,16 +2085,16 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1365,13 +2105,13 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1382,13 +2122,13 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1399,10 +2139,10 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1413,53 +2153,143 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" t="s">
         <v>63</v>
       </c>
-      <c r="G14" t="s">
-        <v>64</v>
+      <c r="H14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>59</v>
-      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="6">
+        <v>1</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="F25" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6">
+        <v>2</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6">
+        <v>3</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6">
+        <v>4</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="6">
+        <v>5</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6">
+        <v>6</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="6">
+        <v>7</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="6">
+        <v>8</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
     <col min="6" max="6" width="45.28515625" customWidth="1"/>
     <col min="7" max="7" width="35.5703125" customWidth="1"/>
     <col min="8" max="8" width="73.140625" customWidth="1"/>
@@ -1473,7 +2303,7 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1497,7 +2327,448 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="14">
+        <v>1</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="14">
+        <f>A18+1</f>
+        <v>2</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="14">
+        <f t="shared" ref="A20:A33" si="0">A19+1</f>
+        <v>3</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="14">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="14">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="14">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="3" width="122.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="C23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>